<commit_message>
retested all sites, updated script to run outside of rcf package, added pdfs of the rcf instructions
</commit_message>
<xml_diff>
--- a/site_testing/rcf_plot_tables_comparisonn.xlsx
+++ b/site_testing/rcf_plot_tables_comparisonn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnchr\Documents\test\site_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnchr\Documents\rcf_addendum\site_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A3A894-24AE-488B-8036-C77BB1ABE297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F9236-0615-46AA-9DA1-E542DA1DC7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E6D3A21A-B011-4B93-BC33-D128C9DF0817}"/>
   </bookViews>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>Site</t>
   </si>
   <si>
-    <t>Future Means</t>
-  </si>
-  <si>
-    <t>Thresholds</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -76,6 +70,30 @@
   </si>
   <si>
     <t>HOCU</t>
+  </si>
+  <si>
+    <t>Comparison of changes in maximum and minimum temperature from historic period to future period. The future means file has 1 output per model and also assigns the climate future (i.e. Hot Wet, Hot Dry, etc.) to each model. No differences means that the change values from historic to future are the same as are the climate future designation.</t>
+  </si>
+  <si>
+    <t>Threshold values compares the outputs of daily data exceeding or not exceeding a threshold value. This compares the data that comes from the calc_thresholds function (SiteName_thresholds.csv) of the rcf package as well as the plot tables script. Any differences are where an observation is different between the two data frames</t>
+  </si>
+  <si>
+    <t>SiteName_mean_diff.txt</t>
+  </si>
+  <si>
+    <t>SiteName_thresholds_diff.txt</t>
+  </si>
+  <si>
+    <t>SiteName_corner_diff.txt</t>
+  </si>
+  <si>
+    <t>This file compares the differences between individual model observations. The corner method selects 4 models, and this compares yearly observations of threshold summary values to the same 4 models between the plot tables script and the cf_quadrant (SiteName_year_summary_c.csv) output.</t>
+  </si>
+  <si>
+    <t>SiteName_quadrant_diff.txt</t>
+  </si>
+  <si>
+    <t>This file compares quadrant values between the two scripts. This averages the yearly threshold observations by quadrant (Hot Wet, Central, etc.) and compares between plot tables output and the output from cf_quadrant (SiteName_year_summary_q.csv)</t>
   </si>
 </sst>
 </file>
@@ -431,191 +449,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F56565-4475-42A9-8497-4679EF0DBEC2}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="36.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.90625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44419</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>44419</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>